<commit_message>
Correccion de columnas fantasmas
</commit_message>
<xml_diff>
--- a/Test/TemplatesTest/WebService1Test/ObtenerProducto - Test2/ObtenerProducto.xlsx
+++ b/Test/TemplatesTest/WebService1Test/ObtenerProducto - Test2/ObtenerProducto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>string</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>HJ5KS987dddDD3434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +391,7 @@
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -402,7 +408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -423,6 +429,12 @@
       </c>
       <c r="G2" t="s">
         <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
permite usar tag especiales para empty y null
</commit_message>
<xml_diff>
--- a/Test/TemplatesTest/WebService1Test/ObtenerProducto - Test2/ObtenerProducto.xlsx
+++ b/Test/TemplatesTest/WebService1Test/ObtenerProducto - Test2/ObtenerProducto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>string</t>
   </si>
@@ -48,19 +48,16 @@
     <t>HJ5KS9876234DD340</t>
   </si>
   <si>
-    <t>HJ5KS98762sdfDD3432HJ5KS9876234DD3431</t>
-  </si>
-  <si>
-    <t>HJ5KS9876234DD3433</t>
-  </si>
-  <si>
-    <t>HJ5KS987dddDD3434</t>
-  </si>
-  <si>
     <t xml:space="preserve">          </t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>${EMPTY}</t>
+  </si>
+  <si>
+    <t>${NULL}</t>
   </si>
 </sst>
 </file>
@@ -381,7 +378,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,22 +416,19 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>